<commit_message>
update report and dashboard
</commit_message>
<xml_diff>
--- a/QuickStart/wwwroot/templates/XuatBaoCaoTheoPhuongTien.xlsx
+++ b/QuickStart/wwwroot/templates/XuatBaoCaoTheoPhuongTien.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Từ ngày :</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Biển Số Xe :</t>
+  </si>
+  <si>
+    <t>Sản Phẩm</t>
   </si>
 </sst>
 </file>
@@ -127,10 +130,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -143,8 +151,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,65 +431,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="28.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" customWidth="1"/>
-    <col min="5" max="5" width="46.5703125" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -491,21 +503,24 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="A1:F2"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="A4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>